<commit_message>
Rename pl to hk
</commit_message>
<xml_diff>
--- a/logs/charts_results_files/data_ws_4.xlsx
+++ b/logs/charts_results_files/data_ws_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joela\crc-p2\logs\charts_results_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA3A774-9592-4DFE-A2EF-EB3DD53921CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9807AD7-6399-4164-8FD1-8ABB6B39C2B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6030" xr2:uid="{7BCBB6FA-6256-42E5-835E-38D250AD9F33}"/>
   </bookViews>
@@ -275,7 +275,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="588838"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -294,7 +294,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="588838"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -2598,7 +2598,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>